<commit_message>
Change to sthlp file (taking out { end p}
</commit_message>
<xml_diff>
--- a/src/import_metadata/prep_demo.xlsx
+++ b/src/import_metadata/prep_demo.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Value Labels" sheetId="2" r:id="rId4"/>
     <sheet name="construct" sheetId="3" r:id="rId5"/>
   </sheets>
-  <calcPr fullCalcOnLoad="true"/>
+  <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
@@ -187,6 +187,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F13"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -311,6 +312,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C6"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -385,6 +387,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D1"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">

</xml_diff>